<commit_message>
Updated sprint 13 Stand-up meeting templet
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint13/Team05 Stand-up Meeting Sprint13.xlsx
+++ b/Project_Files/Sprint13/Team05 Stand-up Meeting Sprint13.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/Sprint13/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Sprint13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_44F963262B534DA529D0775EE74EE392BC082DB2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2A0E957-D41E-46A4-878B-AFE52A4B61A4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09F04CB-B694-441A-A1A0-C797E7909E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="420" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -153,6 +153,24 @@
   </si>
   <si>
     <t>Added toolbar for the event detail page for navigation</t>
+  </si>
+  <si>
+    <t>I have designed blueprint for Item Model class</t>
+  </si>
+  <si>
+    <t>I will write backend code for Item Model class</t>
+  </si>
+  <si>
+    <t>I have written backend code for Item Model class</t>
+  </si>
+  <si>
+    <t>I will add admin functionality.</t>
+  </si>
+  <si>
+    <t>I have added few changes in Item class.</t>
+  </si>
+  <si>
+    <t>I will fix issues.</t>
   </si>
 </sst>
 </file>
@@ -470,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -494,9 +512,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -508,6 +523,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -537,9 +555,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1171,14 +1186,14 @@
       <c r="A14" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>20</v>
+      <c r="B14" s="16" t="s">
+        <v>26</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>22</v>
+      <c r="C14" s="16" t="s">
+        <v>28</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>24</v>
+      <c r="D14" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1205,14 +1220,14 @@
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
       <c r="A15" s="18"/>
-      <c r="B15" s="10" t="s">
-        <v>21</v>
+      <c r="B15" s="16" t="s">
+        <v>27</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>23</v>
+      <c r="C15" s="16" t="s">
+        <v>29</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>25</v>
+      <c r="D15" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1239,13 +1254,13 @@
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
       <c r="A16" s="19"/>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="1"/>
@@ -1275,9 +1290,15 @@
       <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1303,9 +1324,15 @@
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1">
       <c r="A18" s="18"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
+      <c r="B18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1331,9 +1358,15 @@
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1">
       <c r="A19" s="19"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1362,8 +1395,8 @@
         <v>17</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1391,7 +1424,7 @@
       <c r="A21" s="18"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="14"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1500,10 +1533,10 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>

</xml_diff>

<commit_message>
Update the week progress
Update the process of my work
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint13/Team05 Stand-up Meeting Sprint13.xlsx
+++ b/Project_Files/Sprint13/Team05 Stand-up Meeting Sprint13.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Sprint13\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\FreebiesforNewbies\Project_Files\Sprint13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EEBFA3-46B3-4014-88F3-9B7B9324A42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C796B307-EC31-45BD-8AD4-FDA5460F0EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="420" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <r>
       <rPr>
@@ -172,12 +172,30 @@
   <si>
     <t>I have added few changes in Item class</t>
   </si>
+  <si>
+    <t>Accomplishing the Items page</t>
+  </si>
+  <si>
+    <t>We are discussing the queries of Items page</t>
+  </si>
+  <si>
+    <t>Write a backend code in java class code to items</t>
+  </si>
+  <si>
+    <t>We are going to done a queries</t>
+  </si>
+  <si>
+    <t>Write a java class to the items page</t>
+  </si>
+  <si>
+    <t>There are some issues on the Code so we can fix that one</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,8 +240,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF252525"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,8 +266,14 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -413,32 +443,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -484,11 +488,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -512,16 +591,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -534,12 +604,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -555,6 +625,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,7 +859,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -785,12 +870,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A1" s="27"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
+      <c r="A1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -813,12 +898,12 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A2" s="25"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="26"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -841,14 +926,14 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -871,14 +956,14 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -901,14 +986,14 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -993,7 +1078,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="7"/>
@@ -1023,7 +1108,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A9" s="18"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1051,7 +1136,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A10" s="19"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1079,7 +1164,7 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1115,7 +1200,7 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A12" s="18"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
@@ -1149,7 +1234,7 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A13" s="19"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
@@ -1183,16 +1268,16 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="13" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="1"/>
@@ -1219,14 +1304,14 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A15" s="18"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="1"/>
@@ -1253,7 +1338,7 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A16" s="19"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="10" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1372,7 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -1323,7 +1408,7 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A18" s="18"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="10" t="s">
         <v>21</v>
       </c>
@@ -1356,9 +1441,9 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A19" s="19"/>
-      <c r="B19" s="16" t="s">
+    <row r="19" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A19" s="16"/>
+      <c r="B19" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1390,13 +1475,19 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
+      <c r="B20" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1420,11 +1511,17 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A21" s="18"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="13"/>
+    <row r="21" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A21" s="15"/>
+      <c r="B21" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1448,11 +1545,17 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A22" s="19"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+    <row r="22" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
+      <c r="A22" s="16"/>
+      <c r="B22" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>14</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1533,10 +1636,10 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1563,10 +1666,10 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="22"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1593,8 +1696,8 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A27" s="23"/>
-      <c r="B27" s="24"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1621,8 +1724,8 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -28878,6 +28981,6 @@
     <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>